<commit_message>
fixed all values using the right pos-tag-frequencies
</commit_message>
<xml_diff>
--- a/results/formality-score for each collection.xlsx
+++ b/results/formality-score for each collection.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mijn Drive\Studie informatiekunde\master\master project\project\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D024578-78D8-4854-9C6A-892DBAB29876}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1059A3-04C1-4A4F-A1BD-89518B03764F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C4A392A-0A03-4B99-9C84-770D3A655B4A}"/>
   </bookViews>
@@ -936,12 +936,6 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -951,13 +945,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -979,6 +970,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1302,8 +1302,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A516726-32D9-4731-9C44-7E337389D0F9}">
   <dimension ref="A1:CA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BQ19" sqref="BQ19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1316,72 +1317,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="99" t="s">
+      <c r="B1" s="102"/>
+      <c r="C1" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
-      <c r="N1" s="100"/>
-      <c r="O1" s="100"/>
-      <c r="P1" s="100"/>
-      <c r="Q1" s="100"/>
-      <c r="R1" s="100"/>
-      <c r="S1" s="100"/>
-      <c r="T1" s="100"/>
-      <c r="U1" s="100"/>
-      <c r="V1" s="100"/>
-      <c r="W1" s="100"/>
-      <c r="X1" s="100"/>
-      <c r="Y1" s="100"/>
-      <c r="Z1" s="100"/>
-      <c r="AA1" s="100"/>
-      <c r="AB1" s="100"/>
-      <c r="AC1" s="100"/>
-      <c r="AD1" s="100"/>
-      <c r="AE1" s="100"/>
-      <c r="AF1" s="100"/>
-      <c r="AG1" s="100"/>
-      <c r="AH1" s="100"/>
-      <c r="AI1" s="100"/>
-      <c r="AJ1" s="100"/>
-      <c r="AK1" s="100"/>
-      <c r="AL1" s="100"/>
-      <c r="AM1" s="100"/>
-      <c r="AN1" s="100"/>
-      <c r="AO1" s="100"/>
-      <c r="AP1" s="100"/>
-      <c r="AQ1" s="100"/>
-      <c r="AR1" s="100"/>
-      <c r="AS1" s="100"/>
-      <c r="AT1" s="100"/>
-      <c r="AU1" s="100"/>
-      <c r="AV1" s="100"/>
-      <c r="AW1" s="100"/>
-      <c r="AX1" s="100"/>
-      <c r="AY1" s="100"/>
-      <c r="AZ1" s="100"/>
-      <c r="BA1" s="100"/>
-      <c r="BB1" s="100"/>
-      <c r="BC1" s="100"/>
-      <c r="BD1" s="100"/>
-      <c r="BE1" s="100"/>
-      <c r="BF1" s="100"/>
-      <c r="BG1" s="100"/>
-      <c r="BH1" s="100"/>
-      <c r="BI1" s="100"/>
-      <c r="BJ1" s="101"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="107"/>
+      <c r="T1" s="107"/>
+      <c r="U1" s="107"/>
+      <c r="V1" s="107"/>
+      <c r="W1" s="107"/>
+      <c r="X1" s="107"/>
+      <c r="Y1" s="107"/>
+      <c r="Z1" s="107"/>
+      <c r="AA1" s="107"/>
+      <c r="AB1" s="107"/>
+      <c r="AC1" s="107"/>
+      <c r="AD1" s="107"/>
+      <c r="AE1" s="107"/>
+      <c r="AF1" s="107"/>
+      <c r="AG1" s="107"/>
+      <c r="AH1" s="107"/>
+      <c r="AI1" s="107"/>
+      <c r="AJ1" s="107"/>
+      <c r="AK1" s="107"/>
+      <c r="AL1" s="107"/>
+      <c r="AM1" s="107"/>
+      <c r="AN1" s="107"/>
+      <c r="AO1" s="107"/>
+      <c r="AP1" s="107"/>
+      <c r="AQ1" s="107"/>
+      <c r="AR1" s="107"/>
+      <c r="AS1" s="107"/>
+      <c r="AT1" s="107"/>
+      <c r="AU1" s="107"/>
+      <c r="AV1" s="107"/>
+      <c r="AW1" s="107"/>
+      <c r="AX1" s="107"/>
+      <c r="AY1" s="107"/>
+      <c r="AZ1" s="107"/>
+      <c r="BA1" s="107"/>
+      <c r="BB1" s="107"/>
+      <c r="BC1" s="107"/>
+      <c r="BD1" s="107"/>
+      <c r="BE1" s="107"/>
+      <c r="BF1" s="107"/>
+      <c r="BG1" s="107"/>
+      <c r="BH1" s="107"/>
+      <c r="BI1" s="107"/>
+      <c r="BJ1" s="108"/>
       <c r="BK1" s="80"/>
       <c r="BL1" s="80"/>
       <c r="BM1" s="80"/>
@@ -1401,113 +1402,113 @@
       <c r="CA1" s="80"/>
     </row>
     <row r="2" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="106"/>
-      <c r="B2" s="107"/>
-      <c r="C2" s="96" t="s">
+      <c r="A2" s="103"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="97"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="96" t="s">
+      <c r="D2" s="95"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="97"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="96" t="s">
+      <c r="G2" s="95"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="97"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="96" t="s">
+      <c r="J2" s="95"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="97"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="96" t="s">
+      <c r="M2" s="95"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="97"/>
-      <c r="Q2" s="98"/>
-      <c r="R2" s="96" t="s">
+      <c r="P2" s="95"/>
+      <c r="Q2" s="96"/>
+      <c r="R2" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="97"/>
-      <c r="T2" s="98"/>
-      <c r="U2" s="96" t="s">
+      <c r="S2" s="95"/>
+      <c r="T2" s="96"/>
+      <c r="U2" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="V2" s="97"/>
-      <c r="W2" s="98"/>
-      <c r="X2" s="96" t="s">
+      <c r="V2" s="95"/>
+      <c r="W2" s="96"/>
+      <c r="X2" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="Y2" s="97"/>
-      <c r="Z2" s="98"/>
-      <c r="AA2" s="96" t="s">
+      <c r="Y2" s="95"/>
+      <c r="Z2" s="96"/>
+      <c r="AA2" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="AB2" s="97"/>
-      <c r="AC2" s="98"/>
-      <c r="AD2" s="96" t="s">
+      <c r="AB2" s="95"/>
+      <c r="AC2" s="96"/>
+      <c r="AD2" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="AE2" s="97"/>
-      <c r="AF2" s="98"/>
-      <c r="AG2" s="96" t="s">
+      <c r="AE2" s="95"/>
+      <c r="AF2" s="96"/>
+      <c r="AG2" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="AH2" s="97"/>
-      <c r="AI2" s="98"/>
-      <c r="AJ2" s="96" t="s">
+      <c r="AH2" s="95"/>
+      <c r="AI2" s="96"/>
+      <c r="AJ2" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="AK2" s="97"/>
-      <c r="AL2" s="98"/>
-      <c r="AM2" s="96" t="s">
+      <c r="AK2" s="95"/>
+      <c r="AL2" s="96"/>
+      <c r="AM2" s="94" t="s">
         <v>47</v>
       </c>
-      <c r="AN2" s="97"/>
-      <c r="AO2" s="98"/>
-      <c r="AP2" s="96" t="s">
+      <c r="AN2" s="95"/>
+      <c r="AO2" s="96"/>
+      <c r="AP2" s="94" t="s">
         <v>48</v>
       </c>
-      <c r="AQ2" s="97"/>
-      <c r="AR2" s="98"/>
-      <c r="AS2" s="96" t="s">
+      <c r="AQ2" s="95"/>
+      <c r="AR2" s="96"/>
+      <c r="AS2" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="AT2" s="97"/>
-      <c r="AU2" s="98"/>
-      <c r="AV2" s="96" t="s">
+      <c r="AT2" s="95"/>
+      <c r="AU2" s="96"/>
+      <c r="AV2" s="94" t="s">
         <v>50</v>
       </c>
-      <c r="AW2" s="97"/>
-      <c r="AX2" s="98"/>
-      <c r="AY2" s="96" t="s">
+      <c r="AW2" s="95"/>
+      <c r="AX2" s="96"/>
+      <c r="AY2" s="94" t="s">
         <v>51</v>
       </c>
-      <c r="AZ2" s="97"/>
-      <c r="BA2" s="98"/>
-      <c r="BB2" s="96" t="s">
+      <c r="AZ2" s="95"/>
+      <c r="BA2" s="96"/>
+      <c r="BB2" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="BC2" s="97"/>
-      <c r="BD2" s="98"/>
-      <c r="BE2" s="96" t="s">
+      <c r="BC2" s="95"/>
+      <c r="BD2" s="96"/>
+      <c r="BE2" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="BF2" s="97"/>
-      <c r="BG2" s="98"/>
-      <c r="BH2" s="96" t="s">
+      <c r="BF2" s="95"/>
+      <c r="BG2" s="96"/>
+      <c r="BH2" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="BI2" s="97"/>
-      <c r="BJ2" s="98"/>
-      <c r="BK2" s="96" t="s">
+      <c r="BI2" s="95"/>
+      <c r="BJ2" s="96"/>
+      <c r="BK2" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="BL2" s="97"/>
-      <c r="BM2" s="98"/>
+      <c r="BL2" s="95"/>
+      <c r="BM2" s="96"/>
     </row>
     <row r="3" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="46" t="s">
@@ -1736,15 +1737,15 @@
         <v>6.9707068201931248</v>
       </c>
       <c r="I4" s="33">
-        <v>524230</v>
+        <v>534230</v>
       </c>
       <c r="J4" s="7">
         <f>(I4/$I$18)*100</f>
-        <v>7.0363637852289651</v>
+        <v>7.1678331295494973</v>
       </c>
       <c r="K4" s="34">
         <f>(I4/$K$19)*100</f>
-        <v>4.9053885913104729</v>
+        <v>4.9976234089679572</v>
       </c>
       <c r="L4" s="33">
         <v>9528</v>
@@ -1762,11 +1763,11 @@
       </c>
       <c r="P4" s="7">
         <f>(O4/O18)*100</f>
-        <v>9.2794607121818551</v>
+        <v>7.7221647300527883</v>
       </c>
       <c r="Q4" s="34">
         <f>(O4/Q19)*100</f>
-        <v>6.6986959055424009</v>
+        <v>5.8474309943627176</v>
       </c>
       <c r="R4" s="33">
         <v>96872</v>
@@ -1784,11 +1785,11 @@
       </c>
       <c r="V4" s="7">
         <f>(U4/U18)*100</f>
-        <v>7.5438227932521524</v>
+        <v>9.5670713634658391</v>
       </c>
       <c r="W4" s="34">
         <f>(U4/W19)*100</f>
-        <v>5.4012059670342252</v>
+        <v>6.3649572792249893</v>
       </c>
       <c r="X4" s="33">
         <v>13108</v>
@@ -1977,11 +1978,11 @@
       </c>
       <c r="J5" s="7">
         <f t="shared" ref="J5:J11" si="4">(I5/$I$18)*100</f>
-        <v>2.287036342309575</v>
+        <v>2.2861581243604223</v>
       </c>
       <c r="K5" s="34">
         <f t="shared" ref="K5:K16" si="5">(I5/$K$19)*100</f>
-        <v>1.5944033486484612</v>
+        <v>1.5939764713278162</v>
       </c>
       <c r="L5" s="12">
         <v>6238</v>
@@ -1999,11 +2000,11 @@
       </c>
       <c r="P5" s="7">
         <f>(O5/O18)*100</f>
-        <v>9.0221681086623988</v>
+        <v>7.508051439439563</v>
       </c>
       <c r="Q5" s="34">
         <f>(O5/Q19)*100</f>
-        <v>6.5129604449181091</v>
+        <v>5.6852986473325862</v>
       </c>
       <c r="R5" s="12">
         <v>44917</v>
@@ -2021,11 +2022,11 @@
       </c>
       <c r="V5" s="7">
         <f>(U5/U18)*100</f>
-        <v>5.2944306674435957</v>
+        <v>6.7143936718214876</v>
       </c>
       <c r="W5" s="34">
         <f>(U5/W19)*100</f>
-        <v>3.7906922387710846</v>
+        <v>4.4670753727460655</v>
       </c>
       <c r="X5" s="12">
         <v>9614</v>
@@ -2214,11 +2215,11 @@
       </c>
       <c r="J6" s="7">
         <f t="shared" si="4"/>
-        <v>14.909365358186392</v>
+        <v>14.903640188006188</v>
       </c>
       <c r="K6" s="34">
         <f t="shared" si="5"/>
-        <v>10.394037739387183</v>
+        <v>10.391254893387371</v>
       </c>
       <c r="L6" s="14">
         <v>13539</v>
@@ -2236,11 +2237,11 @@
       </c>
       <c r="P6" s="7">
         <f>(O6/O18)*100</f>
-        <v>12.450206905579785</v>
+        <v>10.360790527612691</v>
       </c>
       <c r="Q6" s="34">
         <f>(O6/Q19)*100</f>
-        <v>8.9876074276684328</v>
+        <v>7.8454694732791541</v>
       </c>
       <c r="R6" s="14">
         <v>137845</v>
@@ -2258,11 +2259,11 @@
       </c>
       <c r="V6" s="7">
         <f>(U6/U18)*100</f>
-        <v>10.590194075952226</v>
+        <v>13.430477525030801</v>
       </c>
       <c r="W6" s="34">
         <f>(U6/W19)*100</f>
-        <v>7.582338689907739</v>
+        <v>8.9352752204666501</v>
       </c>
       <c r="X6" s="14">
         <v>27475</v>
@@ -2451,11 +2452,11 @@
       </c>
       <c r="J7" s="7">
         <f t="shared" si="4"/>
-        <v>32.363743351439545</v>
+        <v>32.351315730685471</v>
       </c>
       <c r="K7" s="34">
         <f t="shared" si="5"/>
-        <v>22.56232654450309</v>
+        <v>22.556285823683606</v>
       </c>
       <c r="L7" s="14">
         <v>25310</v>
@@ -2473,11 +2474,11 @@
       </c>
       <c r="P7" s="7">
         <f>(O7/O18)*100</f>
-        <v>23.002282385511034</v>
+        <v>19.14199749937222</v>
       </c>
       <c r="Q7" s="34">
         <f>(O7/Q19)*100</f>
-        <v>16.604983803818836</v>
+        <v>14.494835759749144</v>
       </c>
       <c r="R7" s="14">
         <v>264870</v>
@@ -2491,16 +2492,15 @@
         <v>21.829069493366475</v>
       </c>
       <c r="U7" s="14">
-        <f>U6*2</f>
-        <v>1541558</v>
+        <v>1441036</v>
       </c>
       <c r="V7" s="7">
         <f>(U7/U18)*100</f>
-        <v>21.180388151904452</v>
+        <v>25.109404395761025</v>
       </c>
       <c r="W7" s="34">
         <f>(U7/W19)*100</f>
-        <v>15.164677379815478</v>
+        <v>16.705246591565651</v>
       </c>
       <c r="X7" s="14">
         <v>50624</v>
@@ -2685,15 +2685,15 @@
         <v>0.28594080232688823</v>
       </c>
       <c r="I8" s="35">
-        <v>7860</v>
+        <v>722</v>
       </c>
       <c r="J8" s="7">
         <f t="shared" si="4"/>
-        <v>0.10549914989966172</v>
+        <v>9.6871675486864019E-3</v>
       </c>
       <c r="K8" s="34">
         <f t="shared" si="5"/>
-        <v>7.3548546110867974E-2</v>
+        <v>6.754177229423404E-3</v>
       </c>
       <c r="L8" s="35">
         <v>61</v>
@@ -2711,11 +2711,11 @@
       </c>
       <c r="P8" s="7">
         <f>(O8/O18)*100</f>
-        <v>0.19308763245229776</v>
+        <v>0.16068331462140997</v>
       </c>
       <c r="Q8" s="34">
         <f>(O8/Q19)*100</f>
-        <v>0.13938690760564268</v>
+        <v>0.12167373101191871</v>
       </c>
       <c r="R8" s="35">
         <v>139</v>
@@ -2729,15 +2729,15 @@
         <v>1.1455584473809566E-2</v>
       </c>
       <c r="U8" s="35">
-        <v>1441036</v>
+        <v>2354</v>
       </c>
       <c r="V8" s="7">
         <f>(U8/U18)*100</f>
-        <v>19.799256220568921</v>
+        <v>4.1017391617989729E-2</v>
       </c>
       <c r="W8" s="34">
         <f>(U8/W19)*100</f>
-        <v>14.175818251859337</v>
+        <v>2.7288805051744396E-2</v>
       </c>
       <c r="X8" s="35">
         <v>187</v>
@@ -2926,11 +2926,11 @@
       </c>
       <c r="J9" s="7">
         <f t="shared" si="4"/>
-        <v>4.7352340450320298</v>
+        <v>4.7334157234536391</v>
       </c>
       <c r="K9" s="34">
         <f t="shared" si="5"/>
-        <v>3.3011600552044529</v>
+        <v>3.3002762196551982</v>
       </c>
       <c r="L9" s="2">
         <v>10117</v>
@@ -2944,15 +2944,15 @@
         <v>7.2385790433942692</v>
       </c>
       <c r="O9" s="14">
-        <v>347697</v>
+        <v>3675238</v>
       </c>
       <c r="P9" s="7">
         <f>(O9/O18)*100</f>
-        <v>2.1072187865902885</v>
+        <v>18.535763460846251</v>
       </c>
       <c r="Q9" s="34">
         <f>(O9/Q19)*100</f>
-        <v>1.5211679100363824</v>
+        <v>14.03577902751984</v>
       </c>
       <c r="R9" s="14">
         <v>67724</v>
@@ -2970,11 +2970,11 @@
       </c>
       <c r="V9" s="7">
         <f>(U9/U18)*100</f>
-        <v>7.6555669487360465</v>
+        <v>9.7087852317874681</v>
       </c>
       <c r="W9" s="34">
         <f>(U9/W19)*100</f>
-        <v>5.4812122471288047</v>
+        <v>6.4592392892019808</v>
       </c>
       <c r="X9" s="14">
         <v>14211</v>
@@ -3163,11 +3163,11 @@
       </c>
       <c r="J10" s="7">
         <f t="shared" si="4"/>
-        <v>22.742368525711125</v>
+        <v>22.733635496035976</v>
       </c>
       <c r="K10" s="34">
         <f t="shared" si="5"/>
-        <v>15.854802069727203</v>
+        <v>15.850557186879572</v>
       </c>
       <c r="L10" s="35">
         <v>17710</v>
@@ -3185,11 +3185,11 @@
       </c>
       <c r="P10" s="7">
         <f>(O10/O18)*100</f>
-        <v>18.031554616042879</v>
+        <v>15.005466309182436</v>
       </c>
       <c r="Q10" s="34">
         <f>(O10/Q19)*100</f>
-        <v>13.016694054050271</v>
+        <v>11.362542997781803</v>
       </c>
       <c r="R10" s="35">
         <v>170402</v>
@@ -3207,11 +3207,11 @@
       </c>
       <c r="V10" s="7">
         <f>(U10/U18)*100</f>
-        <v>14.6253080933243</v>
+        <v>18.547806606309187</v>
       </c>
       <c r="W10" s="34">
         <f>(U10/W19)*100</f>
-        <v>10.471388778383883</v>
+        <v>12.339826075021261</v>
       </c>
       <c r="X10" s="35">
         <v>31503</v>
@@ -3400,11 +3400,11 @@
       </c>
       <c r="J11" s="7">
         <f t="shared" si="4"/>
-        <v>15.820389442192706</v>
+        <v>15.814314440360121</v>
       </c>
       <c r="K11" s="34">
         <f t="shared" si="5"/>
-        <v>11.029156571286554</v>
+        <v>11.026203681849815</v>
       </c>
       <c r="L11" s="35">
         <v>16213</v>
@@ -3422,11 +3422,11 @@
       </c>
       <c r="P11" s="7">
         <f>(O11/O18)*100</f>
-        <v>25.914020852979462</v>
+        <v>21.565082718872638</v>
       </c>
       <c r="Q11" s="34">
         <f>(O11/Q19)*100</f>
-        <v>18.70692174558258</v>
+        <v>16.329661111162245</v>
       </c>
       <c r="R11" s="35">
         <v>162204</v>
@@ -3444,11 +3444,11 @@
       </c>
       <c r="V11" s="7">
         <f>(U11/U18)*100</f>
-        <v>13.311033048818304</v>
+        <v>16.881043814206201</v>
       </c>
       <c r="W11" s="34">
         <f>(U11/W19)*100</f>
-        <v>9.5303976645603168</v>
+        <v>11.230931454787759</v>
       </c>
       <c r="X11" s="35">
         <v>38689</v>
@@ -3735,7 +3735,7 @@
       <c r="J13" s="9"/>
       <c r="K13" s="34">
         <f t="shared" si="5"/>
-        <v>14.315251339056084</v>
+        <v>14.311418647572363</v>
       </c>
       <c r="L13" s="14">
         <v>16864</v>
@@ -3751,7 +3751,7 @@
       <c r="P13" s="9"/>
       <c r="Q13" s="34">
         <f>(O13/Q19)*100</f>
-        <v>15.595334344829034</v>
+        <v>13.613491745453207</v>
       </c>
       <c r="R13" s="14">
         <v>140389</v>
@@ -3767,7 +3767,7 @@
       <c r="V13" s="9"/>
       <c r="W13" s="34">
         <f>(U13/W19)*100</f>
-        <v>11.903130328095592</v>
+        <v>14.027037015397656</v>
       </c>
       <c r="X13" s="14">
         <v>26337</v>
@@ -3909,7 +3909,7 @@
       <c r="J14" s="9"/>
       <c r="K14" s="34">
         <f t="shared" si="5"/>
-        <v>5.8898068733081379</v>
+        <v>5.8882299668250155</v>
       </c>
       <c r="L14" s="35">
         <v>14893</v>
@@ -3925,7 +3925,7 @@
       <c r="P14" s="9"/>
       <c r="Q14" s="34">
         <f>(O14/Q19)*100</f>
-        <v>4.5968717132952186</v>
+        <v>4.0127049372687136</v>
       </c>
       <c r="R14" s="35">
         <v>45125</v>
@@ -3941,7 +3941,7 @@
       <c r="V14" s="9"/>
       <c r="W14" s="34">
         <f>(U14/W19)*100</f>
-        <v>10.596626692054619</v>
+        <v>12.487410517295585</v>
       </c>
       <c r="X14" s="35">
         <v>10249</v>
@@ -4083,7 +4083,7 @@
       <c r="J15" s="9"/>
       <c r="K15" s="34">
         <f t="shared" si="5"/>
-        <v>6.292592772461103</v>
+        <v>6.2909080261609311</v>
       </c>
       <c r="L15" s="35">
         <v>3819</v>
@@ -4099,7 +4099,7 @@
       <c r="P15" s="9"/>
       <c r="Q15" s="34">
         <f>(O15/Q19)*100</f>
-        <v>1.5211679100363824</v>
+        <v>1.3278591102213153</v>
       </c>
       <c r="R15" s="35">
         <v>26173</v>
@@ -4115,7 +4115,7 @@
       <c r="V15" s="9"/>
       <c r="W15" s="34">
         <f>(U15/W19)*100</f>
-        <v>2.8110702800032894</v>
+        <v>3.3126569048327852</v>
       </c>
       <c r="X15" s="35">
         <v>3864</v>
@@ -4257,7 +4257,7 @@
       <c r="J16" s="9"/>
       <c r="K16" s="34">
         <f t="shared" si="5"/>
-        <v>3.7875255489963853</v>
+        <v>3.7865114964609328</v>
       </c>
       <c r="L16" s="14">
         <v>5473</v>
@@ -4273,7 +4273,7 @@
       <c r="P16" s="9"/>
       <c r="Q16" s="34">
         <f>(O16/Q19)*100</f>
-        <v>6.098207832616712</v>
+        <v>5.3232524648573536</v>
       </c>
       <c r="R16" s="35">
         <v>56722</v>
@@ -4289,7 +4289,7 @@
       <c r="V16" s="9"/>
       <c r="W16" s="34">
         <f>(U16/W19)*100</f>
-        <v>3.0914414823856333</v>
+        <v>3.6430554744078769</v>
       </c>
       <c r="X16" s="35">
         <v>10238</v>
@@ -4500,7 +4500,7 @@
       </c>
       <c r="I18" s="37">
         <f>SUM(I4:I11)</f>
-        <v>7450297</v>
+        <v>7453159</v>
       </c>
       <c r="J18" s="6">
         <f>SUM(J4:J11)</f>
@@ -4508,7 +4508,7 @@
       </c>
       <c r="K18" s="38">
         <f>SUM(K4:K17)</f>
-        <v>100</v>
+        <v>100.00000000000001</v>
       </c>
       <c r="L18" s="37">
         <f>SUM(L4:L11)</f>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="O18" s="37">
         <f>SUM(O4:O11)</f>
-        <v>16500280</v>
+        <v>19827821</v>
       </c>
       <c r="P18" s="6">
         <f>SUM(P4:P11)</f>
@@ -4532,7 +4532,7 @@
       </c>
       <c r="Q18" s="38">
         <f>SUM(Q4:Q17)</f>
-        <v>99.999999999999986</v>
+        <v>99.999999999999972</v>
       </c>
       <c r="R18" s="37">
         <f>SUM(R4:R11)</f>
@@ -4548,7 +4548,7 @@
       </c>
       <c r="U18" s="37">
         <f>SUM(U4:U11)</f>
-        <v>7278233</v>
+        <v>5739029</v>
       </c>
       <c r="V18" s="6">
         <f>SUM(V4:V11)</f>
@@ -4748,7 +4748,7 @@
       <c r="J19" s="39"/>
       <c r="K19" s="45">
         <f>SUM(I4:I17)</f>
-        <v>10686819</v>
+        <v>10689681</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="39"/>
@@ -4760,7 +4760,7 @@
       <c r="P19" s="39"/>
       <c r="Q19" s="45">
         <f>SUM(O4:O17)</f>
-        <v>22857240</v>
+        <v>26184781</v>
       </c>
       <c r="R19" s="9"/>
       <c r="S19" s="39"/>
@@ -4772,7 +4772,7 @@
       <c r="V19" s="39"/>
       <c r="W19" s="45">
         <f>SUM(U4:U17)</f>
-        <v>10165452</v>
+        <v>8626248</v>
       </c>
       <c r="X19" s="9"/>
       <c r="Y19" s="39"/>
@@ -4931,131 +4931,131 @@
         <v>22</v>
       </c>
       <c r="B21" s="26"/>
-      <c r="C21" s="94">
+      <c r="C21" s="97">
         <f>((D7+D4+D10+D6-D9-D11-D5-D8)+100)/2</f>
         <v>62.555771941928533</v>
       </c>
-      <c r="D21" s="95"/>
+      <c r="D21" s="98"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="94">
+      <c r="F21" s="97">
         <f>((G7+G4+G10+G6-G9-G11-G5-G8)+100)/2</f>
         <v>50.019456097911245</v>
       </c>
-      <c r="G21" s="95"/>
+      <c r="G21" s="98"/>
       <c r="H21" s="51"/>
-      <c r="I21" s="108">
+      <c r="I21" s="105">
         <f>((J7+J4+J10+J6-J9-J11-J5-J8)+100)/2</f>
-        <v>77.05184102056603</v>
-      </c>
-      <c r="J21" s="95"/>
+        <v>77.156424544277144</v>
+      </c>
+      <c r="J21" s="98"/>
       <c r="K21" s="42"/>
-      <c r="L21" s="94">
+      <c r="L21" s="97">
         <f>((M7+M4+M10+M6-M9-M11-M5-M8)+100)/2</f>
         <v>66.946594270432342</v>
       </c>
-      <c r="M21" s="95"/>
+      <c r="M21" s="98"/>
       <c r="N21" s="42"/>
-      <c r="O21" s="94">
+      <c r="O21" s="97">
         <f>((P7+P4+P10+P6-P9-P11-P5-P8)+100)/2</f>
-        <v>62.763504619315555</v>
-      </c>
-      <c r="P21" s="95"/>
+        <v>52.230419066220136</v>
+      </c>
+      <c r="P21" s="98"/>
       <c r="Q21" s="42"/>
-      <c r="R21" s="94">
+      <c r="R21" s="97">
         <f>((S7+S4+S10+S6-S9-S11-S5-S8)+100)/2</f>
         <v>70.900332602095503</v>
       </c>
-      <c r="S21" s="95"/>
+      <c r="S21" s="98"/>
       <c r="T21" s="42"/>
-      <c r="U21" s="94">
+      <c r="U21" s="97">
         <f>((V7+V4+V10+V6-V9-V11-V5-V8)+100)/2</f>
-        <v>53.939713114433133</v>
-      </c>
-      <c r="V21" s="95"/>
+        <v>66.654759890566851</v>
+      </c>
+      <c r="V21" s="98"/>
       <c r="W21" s="42"/>
-      <c r="X21" s="94">
+      <c r="X21" s="97">
         <f>((Y7+Y4+Y10+Y6-Y9-Y11-Y5-Y8)+100)/2</f>
         <v>66.182696819498304</v>
       </c>
-      <c r="Y21" s="95"/>
+      <c r="Y21" s="98"/>
       <c r="Z21" s="42"/>
-      <c r="AA21" s="94">
+      <c r="AA21" s="97">
         <f>((AB7+AB4+AB10+AB6-AB9-AB11-AB5-AB8)+100)/2</f>
         <v>63.867309745591108</v>
       </c>
-      <c r="AB21" s="95"/>
+      <c r="AB21" s="98"/>
       <c r="AC21" s="42"/>
-      <c r="AD21" s="94">
+      <c r="AD21" s="97">
         <f>((AE7+AE4+AE10+AE6-AE9-AE11-AE5-AE8)+100)/2</f>
         <v>63.60886727578005</v>
       </c>
-      <c r="AE21" s="95"/>
+      <c r="AE21" s="98"/>
       <c r="AF21" s="42"/>
-      <c r="AG21" s="94">
+      <c r="AG21" s="97">
         <f>((AH7+AH4+AH10+AH6-AH9-AH11-AH5-AH8)+100)/2</f>
         <v>63.118941231447693</v>
       </c>
-      <c r="AH21" s="95"/>
+      <c r="AH21" s="98"/>
       <c r="AI21" s="42"/>
-      <c r="AJ21" s="94">
+      <c r="AJ21" s="97">
         <f>((AK7+AK4+AK10+AK6-AK9-AK11-AK5-AK8)+100)/2</f>
         <v>73.152326785465903</v>
       </c>
-      <c r="AK21" s="95"/>
+      <c r="AK21" s="98"/>
       <c r="AL21" s="42"/>
-      <c r="AM21" s="94">
+      <c r="AM21" s="97">
         <f>((AN7+AN4+AN10+AN6-AN9-AN11-AN5-AN8)+100)/2</f>
         <v>66.614488145094541</v>
       </c>
-      <c r="AN21" s="95"/>
+      <c r="AN21" s="98"/>
       <c r="AO21" s="42"/>
-      <c r="AP21" s="94">
+      <c r="AP21" s="97">
         <f>((AQ7+AQ4+AQ10+AQ6-AQ9-AQ11-AQ5-AQ8)+100)/2</f>
         <v>66.110814401023333</v>
       </c>
-      <c r="AQ21" s="95"/>
+      <c r="AQ21" s="98"/>
       <c r="AR21" s="42"/>
-      <c r="AS21" s="94">
+      <c r="AS21" s="97">
         <f>((AT7+AT4+AT10+AT6-AT9-AT11-AT5-AT8)+100)/2</f>
         <v>40.524512288406207</v>
       </c>
-      <c r="AT21" s="95"/>
+      <c r="AT21" s="98"/>
       <c r="AU21" s="42"/>
-      <c r="AV21" s="94">
+      <c r="AV21" s="97">
         <f>((AW7+AW4+AW10+AW6-AW9-AW11-AW5-AW8)+100)/2</f>
         <v>58.311562135295404</v>
       </c>
-      <c r="AW21" s="95"/>
+      <c r="AW21" s="98"/>
       <c r="AX21" s="42"/>
-      <c r="AY21" s="94">
+      <c r="AY21" s="97">
         <f>((AZ7+AZ4+AZ10+AZ6-AZ9-AZ11-AZ5-AZ8)+100)/2</f>
         <v>58.321571417219445</v>
       </c>
-      <c r="AZ21" s="95"/>
+      <c r="AZ21" s="98"/>
       <c r="BA21" s="42"/>
-      <c r="BB21" s="94">
+      <c r="BB21" s="97">
         <f>((BC7+BC4+BC10+BC6-BC9-BC11-BC5-BC8)+100)/2</f>
         <v>73.18003543837753</v>
       </c>
-      <c r="BC21" s="95"/>
+      <c r="BC21" s="98"/>
       <c r="BD21" s="42"/>
-      <c r="BE21" s="94">
+      <c r="BE21" s="97">
         <f>((BF7+BF4+BF10+BF6-BF9-BF11-BF5-BF8)+100)/2</f>
         <v>70.45651852836734</v>
       </c>
-      <c r="BF21" s="95"/>
+      <c r="BF21" s="98"/>
       <c r="BG21" s="42"/>
-      <c r="BH21" s="94">
+      <c r="BH21" s="97">
         <f>((BI7+BI4+BI10+BI6-BI9-BI11-BI5-BI8)+100)/2</f>
         <v>64.343705901923983</v>
       </c>
-      <c r="BI21" s="95"/>
+      <c r="BI21" s="98"/>
       <c r="BJ21" s="42"/>
-      <c r="BK21" s="94" t="e">
+      <c r="BK21" s="97" t="e">
         <f>((BL7+BL4+BL10+BL6-BL9-BL11-BL5-BL8)+100)/2</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BL21" s="95"/>
+      <c r="BL21" s="98"/>
       <c r="BM21" s="42"/>
     </row>
     <row r="22" spans="1:65" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5079,7 +5079,7 @@
       <c r="J22" s="41"/>
       <c r="K22" s="43">
         <f>((K7+K4+K10+K6-K9-K11-K5-K8)+100)/2</f>
-        <v>68.859143211838798</v>
+        <v>68.93425538142813</v>
       </c>
       <c r="L22" s="40"/>
       <c r="M22" s="41"/>
@@ -5091,7 +5091,7 @@
       <c r="P22" s="41"/>
       <c r="Q22" s="43">
         <f>((Q7+Q4+Q10+Q6-Q9-Q11-Q5-Q8)+100)/2</f>
-        <v>59.213772091468613</v>
+        <v>51.688933354073114</v>
       </c>
       <c r="R22" s="40"/>
       <c r="S22" s="41"/>
@@ -5103,7 +5103,7 @@
       <c r="V22" s="41"/>
       <c r="W22" s="43">
         <f>((W7+W4+W10+W6-W9-W11-W5-W8)+100)/2</f>
-        <v>52.820745206410891</v>
+        <v>61.080385122245502</v>
       </c>
       <c r="X22" s="40"/>
       <c r="Y22" s="41"/>
@@ -5192,10 +5192,10 @@
     </row>
     <row r="24" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="102" t="s">
+      <c r="A25" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="103"/>
+      <c r="B25" s="100"/>
     </row>
     <row r="26" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A26" s="90" t="s">
@@ -5224,7 +5224,7 @@
         <v>38</v>
       </c>
       <c r="B28" s="92">
-        <v>53.93971311</v>
+        <v>66.650000000000006</v>
       </c>
       <c r="AY28" s="78"/>
       <c r="AZ28" s="79"/>
@@ -5276,7 +5276,7 @@
         <v>42</v>
       </c>
       <c r="B32" s="92">
-        <v>62.763504619999999</v>
+        <v>52.23</v>
       </c>
       <c r="AY32" s="78"/>
       <c r="AZ32" s="79"/>
@@ -5420,7 +5420,7 @@
         <v>41</v>
       </c>
       <c r="B45" s="93">
-        <v>77.051841019999998</v>
+        <v>77.16</v>
       </c>
       <c r="AK45" s="56"/>
       <c r="AL45" s="57"/>
@@ -5465,18 +5465,8 @@
     <mergeCell ref="U2:W2"/>
     <mergeCell ref="U21:V21"/>
     <mergeCell ref="C1:BJ1"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="O21:P21"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="R21:S21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
     <mergeCell ref="X2:Z2"/>
     <mergeCell ref="AJ21:AK21"/>
     <mergeCell ref="AM2:AO2"/>
@@ -5486,11 +5476,22 @@
     <mergeCell ref="AA2:AC2"/>
     <mergeCell ref="AA21:AB21"/>
     <mergeCell ref="AD2:AF2"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
     <mergeCell ref="AG2:AI2"/>
     <mergeCell ref="AD21:AE21"/>
     <mergeCell ref="AG21:AH21"/>
     <mergeCell ref="L21:M21"/>
     <mergeCell ref="F21:G21"/>
+    <mergeCell ref="AJ2:AL2"/>
     <mergeCell ref="BE2:BG2"/>
     <mergeCell ref="BE21:BF21"/>
     <mergeCell ref="BH2:BJ2"/>
@@ -5504,7 +5505,6 @@
     <mergeCell ref="AV21:AW21"/>
     <mergeCell ref="AY21:AZ21"/>
     <mergeCell ref="BB21:BC21"/>
-    <mergeCell ref="AJ2:AL2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5531,11 +5531,11 @@
       <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="97"/>
-      <c r="D1" s="98"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="96"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="46" t="s">
@@ -5760,11 +5760,11 @@
       <c r="A20" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="94" t="e">
+      <c r="B20" s="97" t="e">
         <f>((C6+C3+C9+C5-C8-C10-C4-C7)+100)/2</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C20" s="95"/>
+      <c r="C20" s="98"/>
       <c r="D20" s="42"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>